<commit_message>
Updated DAG to match Sinanovic, et al. study.
</commit_message>
<xml_diff>
--- a/Markov_DAG/Clinical_states.xlsx
+++ b/Markov_DAG/Clinical_states.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshuamusson/Desktop/Analytics/R/Intergrated-CEA-thesis/Markov_DAG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0EB25D5-0F3D-AE47-B96A-7923955B3215}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43D59E98-C555-9D45-92F1-8EBDB92E1011}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{DBD245F2-2450-0C48-9F3A-BADB08A6AFB5}"/>
   </bookViews>
@@ -33,13 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="12">
-  <si>
-    <t>Healthy</t>
-  </si>
-  <si>
-    <t>Exposure</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="15">
   <si>
     <t>Infection</t>
   </si>
@@ -50,12 +44,6 @@
     <t>HSIL</t>
   </si>
   <si>
-    <t>Clearance</t>
-  </si>
-  <si>
-    <t>Carcinoma</t>
-  </si>
-  <si>
     <t>Year 1</t>
   </si>
   <si>
@@ -65,10 +53,31 @@
     <t>Year 3</t>
   </si>
   <si>
-    <t>Reinfection</t>
-  </si>
-  <si>
     <t>Death</t>
+  </si>
+  <si>
+    <t>Well</t>
+  </si>
+  <si>
+    <t>Stage I Cancer</t>
+  </si>
+  <si>
+    <t>Stage II Cancer</t>
+  </si>
+  <si>
+    <t>Stage III Cancer</t>
+  </si>
+  <si>
+    <t>Stage IV Cancer</t>
+  </si>
+  <si>
+    <t>Treatment</t>
+  </si>
+  <si>
+    <t>Year 4</t>
+  </si>
+  <si>
+    <t>Cleared</t>
   </si>
 </sst>
 </file>
@@ -420,164 +429,168 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F176B67-F3F3-1543-8F9F-9A51A8F33690}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B16" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B17" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B19" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -585,7 +598,7 @@
         <v>10</v>
       </c>
       <c r="B20" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -593,7 +606,103 @@
         <v>11</v>
       </c>
       <c r="B21" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>11</v>
+      </c>
+      <c r="B25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>14</v>
+      </c>
+      <c r="B31" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>14</v>
+      </c>
+      <c r="B32" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated DAG and evidence to match original study.
</commit_message>
<xml_diff>
--- a/Markov_DAG/Clinical_states.xlsx
+++ b/Markov_DAG/Clinical_states.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshuamusson/Desktop/Analytics/R/Intergrated-CEA-thesis/Markov_DAG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43D59E98-C555-9D45-92F1-8EBDB92E1011}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C880EFB2-D3F1-714A-A2A9-788FC847F392}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{DBD245F2-2450-0C48-9F3A-BADB08A6AFB5}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{DBD245F2-2450-0C48-9F3A-BADB08A6AFB5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="31">
   <si>
     <t>Infection</t>
   </si>
@@ -44,15 +44,6 @@
     <t>HSIL</t>
   </si>
   <si>
-    <t>Year 1</t>
-  </si>
-  <si>
-    <t>Year 2</t>
-  </si>
-  <si>
-    <t>Year 3</t>
-  </si>
-  <si>
     <t>Death</t>
   </si>
   <si>
@@ -71,13 +62,70 @@
     <t>Stage IV Cancer</t>
   </si>
   <si>
-    <t>Treatment</t>
-  </si>
-  <si>
-    <t>Year 4</t>
-  </si>
-  <si>
-    <t>Cleared</t>
+    <t xml:space="preserve">Infection </t>
+  </si>
+  <si>
+    <t>Detected Stage I: Year 2</t>
+  </si>
+  <si>
+    <t>Detected Stage I: Year 1</t>
+  </si>
+  <si>
+    <t>Detected Stage I: Year 3</t>
+  </si>
+  <si>
+    <t>Detected Stage I: Year 4</t>
+  </si>
+  <si>
+    <t>Detected Stage I: Year 5</t>
+  </si>
+  <si>
+    <t>Detected Stage II: Year 1</t>
+  </si>
+  <si>
+    <t>Detected Stage II: Year 2</t>
+  </si>
+  <si>
+    <t>Detected Stage II: Year 3</t>
+  </si>
+  <si>
+    <t>Detected Stage II: Year 4</t>
+  </si>
+  <si>
+    <t>Detected Stage II: Year 5</t>
+  </si>
+  <si>
+    <t>Detected Stage III: Year 1</t>
+  </si>
+  <si>
+    <t>Detected Stage III: Year 2</t>
+  </si>
+  <si>
+    <t>Detected Stage III: Year 3</t>
+  </si>
+  <si>
+    <t>Detected Stage III: Year 4</t>
+  </si>
+  <si>
+    <t>Detected Stage III: Year 5</t>
+  </si>
+  <si>
+    <t>Detected Stage IV: Year 1</t>
+  </si>
+  <si>
+    <t>Detected Stage IV: Year 2</t>
+  </si>
+  <si>
+    <t>Detected Stage IV: Year 3</t>
+  </si>
+  <si>
+    <t>Detected Stage IV: Year 4</t>
+  </si>
+  <si>
+    <t>Detected Stage IV: Year 5</t>
+  </si>
+  <si>
+    <t>Cancer Survivor</t>
   </si>
 </sst>
 </file>
@@ -429,40 +477,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F176B67-F3F3-1543-8F9F-9A51A8F33690}">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="19.33203125" customWidth="1"/>
+    <col min="1" max="1" width="23.1640625" customWidth="1"/>
+    <col min="2" max="2" width="22" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -470,31 +518,31 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
         <v>0</v>
-      </c>
-      <c r="B6" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
         <v>0</v>
-      </c>
-      <c r="B7" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -502,7 +550,7 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -510,12 +558,12 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B10" t="s">
         <v>2</v>
@@ -526,7 +574,7 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -534,7 +582,7 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -542,167 +590,263 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B18" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B19" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B20" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" t="s">
         <v>11</v>
-      </c>
-      <c r="B21" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B22" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B23" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B24" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B25" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B26" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B27" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B28" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B29" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B30" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B31" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B32" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="B33" t="s">
-        <v>6</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>8</v>
+      </c>
+      <c r="B36" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>25</v>
+      </c>
+      <c r="B37" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>26</v>
+      </c>
+      <c r="B38" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>27</v>
+      </c>
+      <c r="B39" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>28</v>
+      </c>
+      <c r="B40" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>14</v>
+      </c>
+      <c r="B41" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>19</v>
+      </c>
+      <c r="B42" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>24</v>
+      </c>
+      <c r="B43" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>29</v>
+      </c>
+      <c r="B44" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>3</v>
+      </c>
+      <c r="B45" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Squamous Intraepithelial Lesion State transitions (SUB-MOD 5).
</commit_message>
<xml_diff>
--- a/Markov_DAG/Clinical_states.xlsx
+++ b/Markov_DAG/Clinical_states.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshuamusson/Desktop/Analytics/R/Intergrated-CEA-thesis/Markov_DAG/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshuamusson/Desktop/Analytics/R/Dissertation/Markov_DAG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C880EFB2-D3F1-714A-A2A9-788FC847F392}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{429B7C82-77D4-5149-B016-EE8E0089D189}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{DBD245F2-2450-0C48-9F3A-BADB08A6AFB5}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{DBD245F2-2450-0C48-9F3A-BADB08A6AFB5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="31">
   <si>
     <t>Infection</t>
   </si>
@@ -477,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F176B67-F3F3-1543-8F9F-9A51A8F33690}">
-  <dimension ref="A1:B45"/>
+  <dimension ref="A1:B46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -539,10 +539,10 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -566,7 +566,7 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -582,7 +582,7 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -590,12 +590,12 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B14" t="s">
         <v>5</v>
@@ -606,12 +606,12 @@
         <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B16" t="s">
         <v>6</v>
@@ -622,12 +622,12 @@
         <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B18" t="s">
         <v>7</v>
@@ -638,12 +638,12 @@
         <v>7</v>
       </c>
       <c r="B19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B20" t="s">
         <v>8</v>
@@ -651,175 +651,175 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B21" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" t="s">
         <v>11</v>
-      </c>
-      <c r="B22" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" t="s">
         <v>10</v>
-      </c>
-      <c r="B23" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" t="s">
         <v>12</v>
-      </c>
-      <c r="B24" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" t="s">
         <v>13</v>
-      </c>
-      <c r="B25" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B26" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" t="s">
         <v>15</v>
-      </c>
-      <c r="B27" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" t="s">
         <v>16</v>
-      </c>
-      <c r="B28" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" t="s">
         <v>17</v>
-      </c>
-      <c r="B29" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30" t="s">
         <v>18</v>
-      </c>
-      <c r="B30" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="B31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" t="s">
         <v>20</v>
-      </c>
-      <c r="B32" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>20</v>
+      </c>
+      <c r="B33" t="s">
         <v>21</v>
-      </c>
-      <c r="B33" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
+        <v>21</v>
+      </c>
+      <c r="B34" t="s">
         <v>22</v>
-      </c>
-      <c r="B34" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
+        <v>22</v>
+      </c>
+      <c r="B35" t="s">
         <v>23</v>
-      </c>
-      <c r="B35" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B36" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
+        <v>8</v>
+      </c>
+      <c r="B37" t="s">
         <v>25</v>
-      </c>
-      <c r="B37" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
+        <v>25</v>
+      </c>
+      <c r="B38" t="s">
         <v>26</v>
-      </c>
-      <c r="B38" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
+        <v>26</v>
+      </c>
+      <c r="B39" t="s">
         <v>27</v>
-      </c>
-      <c r="B39" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
+        <v>27</v>
+      </c>
+      <c r="B40" t="s">
         <v>28</v>
-      </c>
-      <c r="B40" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="B41" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B42" t="s">
         <v>30</v>
@@ -827,7 +827,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B43" t="s">
         <v>30</v>
@@ -835,7 +835,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B44" t="s">
         <v>30</v>
@@ -843,9 +843,17 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
+        <v>29</v>
+      </c>
+      <c r="B45" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>3</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>